<commit_message>
Add excel category to library files
</commit_message>
<xml_diff>
--- a/atomica/library/cervicalcancer_databook.xlsx
+++ b/atomica/library/cervicalcancer_databook.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A7CC0AAC-A750-FC47-A189-A5EB2FED8BDA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679CA555-6B9C-4B94-A471-B877ABF3BC3C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -26,342 +33,153 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{845BC4E9-381F-9148-9E7A-6C2F2512240A}">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assuming prevalence of 0.5%, taken from a study in Nigeria - https://www.ncbi.nlm.nih.gov/pubmed/29479954</t>
+          <t>Microsoft Office User:
+Assuming prevalence of 0.5%, taken from a study in Nigeria - https://www.ncbi.nlm.nih.gov/pubmed/29479954</t>
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{8853CF8D-7FF1-1842-8E56-1BFE3493BA6C}">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assuming prevalence of 0.5%, taken from a study in Nigeria - https://www.ncbi.nlm.nih.gov/pubmed/29479954</t>
+          <t>Microsoft Office User:
+Assuming prevalence of 0.5%, taken from a study in Nigeria - https://www.ncbi.nlm.nih.gov/pubmed/29479954</t>
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{5E306F34-DD0F-464D-A60F-0C8C001FEFF0}">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
+            <color theme="1"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>9.3% (All women aged 15-49 ever screened, DHS 2010 Armenia)</t>
+          <t>Microsoft Office User:
+9.3% (All women aged 15-49 ever screened, DHS 2010 Armenia)</t>
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{F51DB589-0796-5042-A574-21343020FAA3}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+            <sz val="11"/>
+            <color theme="1"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>9.3% (All women aged 15-49 ever screened, DHS 2010 Armenia)</t>
+          <t>Microsoft Office User:
+9.3% (All women aged 15-49 ever screened, DHS 2010 Armenia)</t>
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{A627974C-8C27-5A48-BA2F-C2619CFBFEBC}">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assume that 80% of those with cervical cancer who received a screening were diagnosed with cervical cancer</t>
+          <t>Microsoft Office User:
+Assume that 80% of those with cervical cancer who received a screening were diagnosed with cervical cancer</t>
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{73B1F9CE-5627-004B-AA61-B2427672973B}">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assume that 80% of those with cervical cancer who received a screening were diagnosed with cervical cancer</t>
+          <t>Microsoft Office User:
+Assume that 80% of those with cervical cancer who received a screening were diagnosed with cervical cancer</t>
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{9675F3D2-A632-3041-94C7-1F6E14855256}">
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assume 50% are treated</t>
+          <t>Microsoft Office User:
+Assume 50% are treated</t>
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{DC2C1505-DF38-2F42-A5A1-188C166B452A}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assume 50% are treated</t>
+          <t>Microsoft Office User:
+Assume 50% are treated</t>
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{F0289E20-6DD0-E141-A304-BC6BD34C2399}">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">From </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>http://www.hpvcentre.net/statistics/reports/ARM.pdf</t>
+          <t>Microsoft Office User:
+From http://www.hpvcentre.net/statistics/reports/ARM.pdf</t>
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{95D6FA0E-3F23-D94A-B82A-B05390AB8E0F}">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>From http://www.hpvcentre.net/statistics/reports/ARM.pdf</t>
+          <t>Microsoft Office User:
+From http://www.hpvcentre.net/statistics/reports/ARM.pdf</t>
         </r>
       </text>
     </comment>
@@ -378,6 +196,12 @@
     <t>Full Name</t>
   </si>
   <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>Women 30-64</t>
+  </si>
+  <si>
     <t>Population size</t>
   </si>
   <si>
@@ -393,9 +217,24 @@
     <t>OR</t>
   </si>
   <si>
+    <t>Estimated number of women with cervical cancer</t>
+  </si>
+  <si>
+    <t>Estimated number of women with cervical cancer who have ever been screened</t>
+  </si>
+  <si>
+    <t>Estimated number of women with cervical cancer who have ever been diagnosed</t>
+  </si>
+  <si>
+    <t>Estimated number of women being treated for cervical cancer</t>
+  </si>
+  <si>
     <t>Annual number of births</t>
   </si>
   <si>
+    <t>Estimated number of new cervical cancer cases annually</t>
+  </si>
+  <si>
     <t>Annual number screened</t>
   </si>
   <si>
@@ -409,27 +248,6 @@
   </si>
   <si>
     <t>Probability</t>
-  </si>
-  <si>
-    <t>Estimated number of women with cervical cancer</t>
-  </si>
-  <si>
-    <t>women</t>
-  </si>
-  <si>
-    <t>Women 30-64</t>
-  </si>
-  <si>
-    <t>Estimated number of new cervical cancer cases annually</t>
-  </si>
-  <si>
-    <t>Estimated number of women with cervical cancer who have ever been screened</t>
-  </si>
-  <si>
-    <t>Estimated number of women being treated for cervical cancer</t>
-  </si>
-  <si>
-    <t>Estimated number of women with cervical cancer who have ever been diagnosed</t>
   </si>
   <si>
     <t>Mortality rate for those with untreated cervical cancer</t>
@@ -439,7 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,25 +272,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -553,19 +352,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp"/>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -1053,12 +840,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.83203125" customWidth="1"/>
+    <col min="1" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1066,12 +853,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1090,23 +877,23 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.5" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="3.83203125" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1">
@@ -1122,17 +909,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
         <f>F2/1.01</f>
@@ -1144,15 +931,15 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1">
@@ -1168,17 +955,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
         <f>5/1000*E2</f>
@@ -1191,15 +978,15 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1">
@@ -1215,17 +1002,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
         <f>E5*0.093</f>
@@ -1238,15 +1025,15 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -1262,17 +1049,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
         <f>E8*0.9</f>
@@ -1285,15 +1072,15 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1">
@@ -1309,17 +1096,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2">
         <f>E11*0.5</f>
@@ -1332,15 +1119,15 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
@@ -1356,17 +1143,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E17" s="2">
         <f>13/1000*E2</f>
@@ -1379,15 +1166,15 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
@@ -1403,17 +1190,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E20" s="2">
         <v>272</v>
@@ -1424,15 +1211,15 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1">
@@ -1448,17 +1235,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2">
         <f>0.093*E2</f>
@@ -1471,15 +1258,15 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1">
@@ -1495,17 +1282,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E26" s="2">
         <f>200</f>
@@ -1518,15 +1305,15 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1">
@@ -1542,17 +1329,17 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E29" s="2">
         <v>80</v>
@@ -1563,15 +1350,15 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
@@ -1587,34 +1374,34 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C32" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1">
@@ -1630,19 +1417,19 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>women</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C35" s="4">
         <v>0.05</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1651,66 +1438,66 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="23" priority="9">
       <formula>COUNTIF(E11:H11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="10">
+    <cfRule type="expression" dxfId="22" priority="10">
       <formula>AND(COUNTIF(E11:H11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="23" priority="11">
+    <cfRule type="expression" dxfId="21" priority="11">
       <formula>COUNTIF(E14:H14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="12">
+    <cfRule type="expression" dxfId="20" priority="12">
       <formula>AND(COUNTIF(E14:H14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="19" priority="13">
       <formula>COUNTIF(E17:H17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>AND(COUNTIF(E17:H17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>COUNTIF(E2:H2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>AND(COUNTIF(E2:H2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>COUNTIF(E20:H20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>AND(COUNTIF(E20:H20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>COUNTIF(E23:H23,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>AND(COUNTIF(E23:H23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="13" priority="19">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>COUNTIF(E26:H26,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>AND(COUNTIF(E26:H26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>COUNTIF(E29:H29,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22">
+    <cfRule type="expression" dxfId="8" priority="22">
       <formula>AND(COUNTIF(E29:H29,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C29)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1747,10 +1534,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B29 B26 B23 B20 B17 B14 B11 B8 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2 B29 B26 B23 B20 B17 B14 B11 B8 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32 B35" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B32 B35" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>